<commit_message>
Versione 0,1. Prima release
</commit_message>
<xml_diff>
--- a/sheetjs.xlsx
+++ b/sheetjs.xlsx
@@ -10,8 +10,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -375,46 +377,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>city</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>John</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Seattle</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Mike</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Los Angeles</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Zach</v>
-      </c>
-      <c r="B4" t="str">
-        <v>New York</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>